<commit_message>
31 Nov 2021 2nd commit
</commit_message>
<xml_diff>
--- a/src/main/java/ccpa/testdata/TestDataCCPA.xlsx
+++ b/src/main/java/ccpa/testdata/TestDataCCPA.xlsx
@@ -1333,8 +1333,8 @@
   <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1411,7 +1411,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -1425,7 +1425,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>8</v>
@@ -1439,7 +1439,7 @@
         <v>201</v>
       </c>
       <c r="C7" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1453,7 +1453,7 @@
         <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1467,7 +1467,7 @@
         <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
         <v>113</v>
@@ -1481,7 +1481,7 @@
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
         <v>114</v>
@@ -1495,7 +1495,7 @@
         <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
         <v>115</v>
@@ -1509,7 +1509,7 @@
         <v>200</v>
       </c>
       <c r="C12" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
         <v>116</v>
@@ -1523,7 +1523,7 @@
         <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
         <v>117</v>
@@ -1537,7 +1537,7 @@
         <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D14" t="s">
         <v>118</v>
@@ -1551,7 +1551,7 @@
         <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D15" t="s">
         <v>119</v>
@@ -1565,7 +1565,7 @@
         <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D16" t="s">
         <v>120</v>
@@ -1579,7 +1579,7 @@
         <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D17" t="s">
         <v>121</v>
@@ -1593,7 +1593,7 @@
         <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D18" t="s">
         <v>122</v>
@@ -1607,7 +1607,7 @@
         <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D19" t="s">
         <v>123</v>
@@ -1621,7 +1621,7 @@
         <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
         <v>124</v>
@@ -1635,7 +1635,7 @@
         <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D21" t="s">
         <v>125</v>
@@ -1649,7 +1649,7 @@
         <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D22" t="s">
         <v>126</v>
@@ -1663,7 +1663,7 @@
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D23" t="s">
         <v>127</v>
@@ -1677,7 +1677,7 @@
         <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D24" t="s">
         <v>128</v>
@@ -1691,7 +1691,7 @@
         <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D25" t="s">
         <v>129</v>
@@ -1705,7 +1705,7 @@
         <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D26" t="s">
         <v>130</v>
@@ -1719,7 +1719,7 @@
         <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D27" t="s">
         <v>131</v>
@@ -1733,7 +1733,7 @@
         <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D28" t="s">
         <v>132</v>
@@ -1747,7 +1747,7 @@
         <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D29" t="s">
         <v>133</v>
@@ -1761,7 +1761,7 @@
         <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D30" t="s">
         <v>134</v>
@@ -1775,7 +1775,7 @@
         <v>51</v>
       </c>
       <c r="C31" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D31" t="s">
         <v>135</v>
@@ -1789,7 +1789,7 @@
         <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D32" t="s">
         <v>136</v>
@@ -1803,7 +1803,7 @@
         <v>53</v>
       </c>
       <c r="C33" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D33" t="s">
         <v>137</v>
@@ -1817,7 +1817,7 @@
         <v>54</v>
       </c>
       <c r="C34" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D34" t="s">
         <v>138</v>
@@ -1831,7 +1831,7 @@
         <v>55</v>
       </c>
       <c r="C35" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D35" t="s">
         <v>139</v>
@@ -1845,7 +1845,7 @@
         <v>56</v>
       </c>
       <c r="C36" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D36" t="s">
         <v>140</v>
@@ -1859,7 +1859,7 @@
         <v>57</v>
       </c>
       <c r="C37" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D37" t="s">
         <v>141</v>
@@ -1873,7 +1873,7 @@
         <v>58</v>
       </c>
       <c r="C38" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D38" t="s">
         <v>142</v>
@@ -1887,7 +1887,7 @@
         <v>59</v>
       </c>
       <c r="C39" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D39" t="s">
         <v>143</v>
@@ -1901,7 +1901,7 @@
         <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D40" t="s">
         <v>144</v>
@@ -1915,7 +1915,7 @@
         <v>61</v>
       </c>
       <c r="C41" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D41" t="s">
         <v>145</v>
@@ -1929,7 +1929,7 @@
         <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D42" t="s">
         <v>146</v>
@@ -1943,7 +1943,7 @@
         <v>63</v>
       </c>
       <c r="C43" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D43" t="s">
         <v>147</v>
@@ -1957,7 +1957,7 @@
         <v>64</v>
       </c>
       <c r="C44" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D44" t="s">
         <v>148</v>
@@ -1971,7 +1971,7 @@
         <v>65</v>
       </c>
       <c r="C45" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D45" t="s">
         <v>149</v>
@@ -1985,7 +1985,7 @@
         <v>66</v>
       </c>
       <c r="C46" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D46" t="s">
         <v>150</v>
@@ -1999,7 +1999,7 @@
         <v>67</v>
       </c>
       <c r="C47" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D47" t="s">
         <v>151</v>
@@ -2013,7 +2013,7 @@
         <v>68</v>
       </c>
       <c r="C48" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D48" t="s">
         <v>152</v>
@@ -2027,7 +2027,7 @@
         <v>69</v>
       </c>
       <c r="C49" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D49" t="s">
         <v>153</v>
@@ -2041,7 +2041,7 @@
         <v>70</v>
       </c>
       <c r="C50" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D50" t="s">
         <v>154</v>
@@ -2055,7 +2055,7 @@
         <v>71</v>
       </c>
       <c r="C51" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D51" t="s">
         <v>155</v>
@@ -2069,7 +2069,7 @@
         <v>72</v>
       </c>
       <c r="C52" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D52" t="s">
         <v>156</v>
@@ -2083,7 +2083,7 @@
         <v>73</v>
       </c>
       <c r="C53" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D53" t="s">
         <v>157</v>
@@ -2097,7 +2097,7 @@
         <v>74</v>
       </c>
       <c r="C54" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D54" t="s">
         <v>158</v>
@@ -2111,7 +2111,7 @@
         <v>75</v>
       </c>
       <c r="C55" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D55" t="s">
         <v>159</v>
@@ -2125,7 +2125,7 @@
         <v>76</v>
       </c>
       <c r="C56" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D56" t="s">
         <v>160</v>
@@ -2139,7 +2139,7 @@
         <v>77</v>
       </c>
       <c r="C57" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D57" t="s">
         <v>161</v>
@@ -2153,7 +2153,7 @@
         <v>78</v>
       </c>
       <c r="C58" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D58" t="s">
         <v>162</v>
@@ -2167,7 +2167,7 @@
         <v>79</v>
       </c>
       <c r="C59" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D59" t="s">
         <v>163</v>
@@ -2181,7 +2181,7 @@
         <v>80</v>
       </c>
       <c r="C60" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D60" t="s">
         <v>164</v>
@@ -2195,7 +2195,7 @@
         <v>81</v>
       </c>
       <c r="C61" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D61" t="s">
         <v>165</v>
@@ -2209,7 +2209,7 @@
         <v>82</v>
       </c>
       <c r="C62" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D62" t="s">
         <v>166</v>
@@ -2223,7 +2223,7 @@
         <v>83</v>
       </c>
       <c r="C63" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D63" t="s">
         <v>167</v>
@@ -2237,7 +2237,7 @@
         <v>84</v>
       </c>
       <c r="C64" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D64" t="s">
         <v>168</v>
@@ -2251,7 +2251,7 @@
         <v>85</v>
       </c>
       <c r="C65" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D65" t="s">
         <v>169</v>
@@ -2265,7 +2265,7 @@
         <v>86</v>
       </c>
       <c r="C66" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D66" t="s">
         <v>170</v>
@@ -2279,7 +2279,7 @@
         <v>87</v>
       </c>
       <c r="C67" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D67" t="s">
         <v>171</v>
@@ -2293,7 +2293,7 @@
         <v>88</v>
       </c>
       <c r="C68" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D68" t="s">
         <v>172</v>
@@ -2307,7 +2307,7 @@
         <v>89</v>
       </c>
       <c r="C69" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D69" t="s">
         <v>173</v>
@@ -2321,7 +2321,7 @@
         <v>90</v>
       </c>
       <c r="C70" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D70" t="s">
         <v>174</v>
@@ -2335,7 +2335,7 @@
         <v>91</v>
       </c>
       <c r="C71" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D71" t="s">
         <v>175</v>
@@ -2349,7 +2349,7 @@
         <v>92</v>
       </c>
       <c r="C72" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D72" t="s">
         <v>176</v>
@@ -2363,7 +2363,7 @@
         <v>93</v>
       </c>
       <c r="C73" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D73" t="s">
         <v>177</v>
@@ -2377,7 +2377,7 @@
         <v>94</v>
       </c>
       <c r="C74" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D74" t="s">
         <v>178</v>
@@ -2391,7 +2391,7 @@
         <v>95</v>
       </c>
       <c r="C75" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D75" t="s">
         <v>179</v>
@@ -2405,7 +2405,7 @@
         <v>96</v>
       </c>
       <c r="C76" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D76" t="s">
         <v>180</v>
@@ -2419,7 +2419,7 @@
         <v>97</v>
       </c>
       <c r="C77" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D77" t="s">
         <v>181</v>
@@ -2433,7 +2433,7 @@
         <v>98</v>
       </c>
       <c r="C78" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D78" t="s">
         <v>182</v>
@@ -2447,7 +2447,7 @@
         <v>99</v>
       </c>
       <c r="C79" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D79" t="s">
         <v>183</v>
@@ -2461,7 +2461,7 @@
         <v>100</v>
       </c>
       <c r="C80" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D80" t="s">
         <v>184</v>
@@ -2475,7 +2475,7 @@
         <v>101</v>
       </c>
       <c r="C81" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D81" t="s">
         <v>185</v>
@@ -2489,7 +2489,7 @@
         <v>102</v>
       </c>
       <c r="C82" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D82" t="s">
         <v>186</v>
@@ -2503,7 +2503,7 @@
         <v>103</v>
       </c>
       <c r="C83" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D83" t="s">
         <v>187</v>
@@ -2517,7 +2517,7 @@
         <v>104</v>
       </c>
       <c r="C84" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D84" t="s">
         <v>188</v>
@@ -2531,7 +2531,7 @@
         <v>105</v>
       </c>
       <c r="C85" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D85" t="s">
         <v>189</v>
@@ -2545,7 +2545,7 @@
         <v>106</v>
       </c>
       <c r="C86" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D86" t="s">
         <v>190</v>
@@ -2559,7 +2559,7 @@
         <v>107</v>
       </c>
       <c r="C87" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D87" t="s">
         <v>191</v>
@@ -2573,7 +2573,7 @@
         <v>108</v>
       </c>
       <c r="C88" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D88" t="s">
         <v>192</v>
@@ -2587,7 +2587,7 @@
         <v>109</v>
       </c>
       <c r="C89" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D89" t="s">
         <v>193</v>
@@ -2601,7 +2601,7 @@
         <v>110</v>
       </c>
       <c r="C90" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D90" t="s">
         <v>194</v>
@@ -2615,7 +2615,7 @@
         <v>111</v>
       </c>
       <c r="C91" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D91" t="s">
         <v>195</v>

</xml_diff>

<commit_message>
18 Nov 2021 commit
</commit_message>
<xml_diff>
--- a/src/main/java/ccpa/testdata/TestDataCCPA.xlsx
+++ b/src/main/java/ccpa/testdata/TestDataCCPA.xlsx
@@ -994,7 +994,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1333,8 +1333,8 @@
   <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H91" sqref="H91"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G88" sqref="G88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1439,7 +1439,7 @@
         <v>201</v>
       </c>
       <c r="C7" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1523,7 +1523,7 @@
         <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="D13" t="s">
         <v>117</v>
@@ -1621,7 +1621,7 @@
         <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="D20" t="s">
         <v>124</v>
@@ -1859,7 +1859,7 @@
         <v>57</v>
       </c>
       <c r="C37" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="D37" t="s">
         <v>141</v>
@@ -1943,7 +1943,7 @@
         <v>63</v>
       </c>
       <c r="C43" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="D43" t="s">
         <v>147</v>
@@ -1999,7 +1999,7 @@
         <v>67</v>
       </c>
       <c r="C47" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="D47" t="s">
         <v>151</v>
@@ -2097,7 +2097,7 @@
         <v>74</v>
       </c>
       <c r="C54" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="D54" t="s">
         <v>158</v>
@@ -2265,7 +2265,7 @@
         <v>86</v>
       </c>
       <c r="C66" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="D66" t="s">
         <v>170</v>
@@ -2545,7 +2545,7 @@
         <v>106</v>
       </c>
       <c r="C86" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="D86" t="s">
         <v>190</v>
@@ -2559,7 +2559,7 @@
         <v>107</v>
       </c>
       <c r="C87" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="D87" t="s">
         <v>191</v>
@@ -2573,7 +2573,7 @@
         <v>108</v>
       </c>
       <c r="C88" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="D88" t="s">
         <v>192</v>

</xml_diff>

<commit_message>
18 nov 2021 commit 3rd
</commit_message>
<xml_diff>
--- a/src/main/java/ccpa/testdata/TestDataCCPA.xlsx
+++ b/src/main/java/ccpa/testdata/TestDataCCPA.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="201">
   <si>
     <t>ON</t>
   </si>
@@ -212,9 +212,6 @@
     <t>www.hemlibra-hcp.com</t>
   </si>
   <si>
-    <t>www.her2treatment.com</t>
-  </si>
-  <si>
     <t>www.her2treatmentoptions.com</t>
   </si>
   <si>
@@ -614,9 +611,6 @@
     <t>URL91</t>
   </si>
   <si>
-    <t>OFF</t>
-  </si>
-  <si>
     <t>HER2+ Breast Cancer Treatment | PERJETA® (pertuzumab)</t>
   </si>
   <si>
@@ -627,6 +621,9 @@
   </si>
   <si>
     <t>https://www.actemrainfo.com/</t>
+  </si>
+  <si>
+    <t>https://www.her2treatment.com</t>
   </si>
 </sst>
 </file>
@@ -1333,8 +1330,8 @@
   <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G88" sqref="G88"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1366,7 +1363,7 @@
         <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -1380,7 +1377,7 @@
         <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -1391,10 +1388,10 @@
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -1436,10 +1433,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C7" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1470,7 +1467,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>20</v>
@@ -1484,7 +1481,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>20</v>
@@ -1498,7 +1495,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>20</v>
@@ -1506,13 +1503,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>20</v>
@@ -1523,10 +1520,10 @@
         <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>20</v>
@@ -1540,7 +1537,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>20</v>
@@ -1554,7 +1551,7 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>20</v>
@@ -1568,7 +1565,7 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>20</v>
@@ -1582,7 +1579,7 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>20</v>
@@ -1596,7 +1593,7 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>20</v>
@@ -1610,7 +1607,7 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>20</v>
@@ -1621,10 +1618,10 @@
         <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>20</v>
@@ -1638,7 +1635,7 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>20</v>
@@ -1652,7 +1649,7 @@
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>20</v>
@@ -1666,7 +1663,7 @@
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>20</v>
@@ -1680,7 +1677,7 @@
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>20</v>
@@ -1694,7 +1691,7 @@
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>20</v>
@@ -1708,7 +1705,7 @@
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>20</v>
@@ -1722,7 +1719,7 @@
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>20</v>
@@ -1736,7 +1733,7 @@
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>20</v>
@@ -1750,7 +1747,7 @@
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>20</v>
@@ -1764,7 +1761,7 @@
         <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>20</v>
@@ -1778,7 +1775,7 @@
         <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>20</v>
@@ -1792,7 +1789,7 @@
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>20</v>
@@ -1806,7 +1803,7 @@
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>20</v>
@@ -1820,7 +1817,7 @@
         <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>20</v>
@@ -1834,7 +1831,7 @@
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>20</v>
@@ -1848,7 +1845,7 @@
         <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>20</v>
@@ -1859,10 +1856,10 @@
         <v>57</v>
       </c>
       <c r="C37" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>20</v>
@@ -1876,7 +1873,7 @@
         <v>0</v>
       </c>
       <c r="D38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>20</v>
@@ -1890,7 +1887,7 @@
         <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>20</v>
@@ -1904,7 +1901,7 @@
         <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>20</v>
@@ -1918,7 +1915,7 @@
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>20</v>
@@ -1932,7 +1929,7 @@
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>20</v>
@@ -1940,13 +1937,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>63</v>
+        <v>200</v>
       </c>
       <c r="C43" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D43" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>20</v>
@@ -1954,13 +1951,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C44" t="s">
         <v>0</v>
       </c>
       <c r="D44" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>20</v>
@@ -1968,13 +1965,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C45" t="s">
         <v>0</v>
       </c>
       <c r="D45" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>20</v>
@@ -1982,13 +1979,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C46" t="s">
         <v>0</v>
       </c>
       <c r="D46" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>20</v>
@@ -1996,13 +1993,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C47" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D47" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>20</v>
@@ -2010,13 +2007,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C48" t="s">
         <v>0</v>
       </c>
       <c r="D48" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>20</v>
@@ -2024,13 +2021,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C49" t="s">
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>20</v>
@@ -2038,13 +2035,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C50" t="s">
         <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>20</v>
@@ -2052,13 +2049,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C51" t="s">
         <v>0</v>
       </c>
       <c r="D51" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>20</v>
@@ -2066,13 +2063,13 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C52" t="s">
         <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>20</v>
@@ -2080,13 +2077,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C53" t="s">
         <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>20</v>
@@ -2094,13 +2091,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C54" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>20</v>
@@ -2108,13 +2105,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C55" t="s">
         <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>20</v>
@@ -2122,13 +2119,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C56" t="s">
         <v>0</v>
       </c>
       <c r="D56" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>20</v>
@@ -2136,13 +2133,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C57" t="s">
         <v>0</v>
       </c>
       <c r="D57" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>20</v>
@@ -2150,13 +2147,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C58" t="s">
         <v>0</v>
       </c>
       <c r="D58" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>20</v>
@@ -2164,13 +2161,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C59" t="s">
         <v>0</v>
       </c>
       <c r="D59" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E59" s="6" t="s">
         <v>20</v>
@@ -2178,13 +2175,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C60" t="s">
         <v>0</v>
       </c>
       <c r="D60" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>20</v>
@@ -2192,13 +2189,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C61" t="s">
         <v>0</v>
       </c>
       <c r="D61" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>20</v>
@@ -2206,13 +2203,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C62" t="s">
         <v>0</v>
       </c>
       <c r="D62" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E62" s="6" t="s">
         <v>20</v>
@@ -2220,13 +2217,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C63" t="s">
         <v>0</v>
       </c>
       <c r="D63" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>20</v>
@@ -2234,13 +2231,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C64" t="s">
         <v>0</v>
       </c>
       <c r="D64" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>20</v>
@@ -2248,13 +2245,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C65" t="s">
         <v>0</v>
       </c>
       <c r="D65" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>20</v>
@@ -2262,13 +2259,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C66" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D66" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>20</v>
@@ -2276,13 +2273,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C67" t="s">
         <v>0</v>
       </c>
       <c r="D67" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>20</v>
@@ -2290,13 +2287,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C68" t="s">
         <v>0</v>
       </c>
       <c r="D68" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>20</v>
@@ -2304,13 +2301,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C69" t="s">
         <v>0</v>
       </c>
       <c r="D69" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E69" s="6" t="s">
         <v>20</v>
@@ -2318,13 +2315,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C70" t="s">
         <v>0</v>
       </c>
       <c r="D70" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>20</v>
@@ -2332,13 +2329,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C71" t="s">
         <v>0</v>
       </c>
       <c r="D71" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E71" s="6" t="s">
         <v>20</v>
@@ -2346,13 +2343,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C72" t="s">
         <v>0</v>
       </c>
       <c r="D72" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E72" s="6" t="s">
         <v>20</v>
@@ -2360,13 +2357,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C73" t="s">
         <v>0</v>
       </c>
       <c r="D73" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E73" s="6" t="s">
         <v>20</v>
@@ -2374,13 +2371,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C74" t="s">
         <v>0</v>
       </c>
       <c r="D74" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E74" s="6" t="s">
         <v>20</v>
@@ -2388,13 +2385,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C75" t="s">
         <v>0</v>
       </c>
       <c r="D75" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E75" s="6" t="s">
         <v>20</v>
@@ -2402,13 +2399,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C76" t="s">
         <v>0</v>
       </c>
       <c r="D76" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>20</v>
@@ -2416,13 +2413,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C77" t="s">
         <v>0</v>
       </c>
       <c r="D77" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E77" s="6" t="s">
         <v>20</v>
@@ -2430,13 +2427,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C78" t="s">
         <v>0</v>
       </c>
       <c r="D78" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E78" s="6" t="s">
         <v>20</v>
@@ -2444,13 +2441,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C79" t="s">
         <v>0</v>
       </c>
       <c r="D79" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E79" s="6" t="s">
         <v>20</v>
@@ -2458,13 +2455,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C80" t="s">
         <v>0</v>
       </c>
       <c r="D80" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E80" s="6" t="s">
         <v>20</v>
@@ -2472,13 +2469,13 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C81" t="s">
         <v>0</v>
       </c>
       <c r="D81" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E81" s="6" t="s">
         <v>20</v>
@@ -2486,13 +2483,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C82" t="s">
         <v>0</v>
       </c>
       <c r="D82" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E82" s="6" t="s">
         <v>20</v>
@@ -2500,13 +2497,13 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C83" t="s">
         <v>0</v>
       </c>
       <c r="D83" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E83" s="6" t="s">
         <v>20</v>
@@ -2514,13 +2511,13 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C84" t="s">
         <v>0</v>
       </c>
       <c r="D84" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E84" s="6" t="s">
         <v>20</v>
@@ -2528,13 +2525,13 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C85" t="s">
         <v>0</v>
       </c>
       <c r="D85" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E85" s="6" t="s">
         <v>20</v>
@@ -2542,13 +2539,13 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C86" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D86" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E86" s="6" t="s">
         <v>20</v>
@@ -2556,13 +2553,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C87" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D87" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E87" s="6" t="s">
         <v>20</v>
@@ -2570,13 +2567,13 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C88" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D88" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E88" s="6" t="s">
         <v>20</v>
@@ -2584,13 +2581,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C89" t="s">
         <v>0</v>
       </c>
       <c r="D89" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E89" s="6" t="s">
         <v>20</v>
@@ -2598,13 +2595,13 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C90" t="s">
         <v>0</v>
       </c>
       <c r="D90" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E90" s="6" t="s">
         <v>20</v>
@@ -2612,13 +2609,13 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C91" t="s">
         <v>0</v>
       </c>
       <c r="D91" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E91" s="6" t="s">
         <v>20</v>
@@ -2626,13 +2623,13 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C92" t="s">
         <v>0</v>
       </c>
       <c r="D92" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E92" s="6" t="s">
         <v>20</v>
@@ -2670,7 +2667,7 @@
     <hyperlink ref="A39" r:id="rId28" display="http://www.genentech-pro.com/"/>
     <hyperlink ref="A40" r:id="rId29" display="http://www.hemework.com/"/>
     <hyperlink ref="A41" r:id="rId30" display="http://www.hemlibra.com/"/>
-    <hyperlink ref="A43" r:id="rId31" display="http://www.her2treatment.com/"/>
+    <hyperlink ref="A43" r:id="rId31"/>
     <hyperlink ref="A44" r:id="rId32" display="http://www.her2treatmentoptions.com/"/>
     <hyperlink ref="A45" r:id="rId33" display="http://www.herceptin.com/"/>
     <hyperlink ref="A46" r:id="rId34" display="http://www.herceptinhylecta.com/"/>

</xml_diff>

<commit_message>
18 Nov 221 commit 5th
</commit_message>
<xml_diff>
--- a/src/main/java/ccpa/testdata/TestDataCCPA.xlsx
+++ b/src/main/java/ccpa/testdata/TestDataCCPA.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="202">
   <si>
     <t>ON</t>
   </si>
@@ -212,6 +212,9 @@
     <t>www.hemlibra-hcp.com</t>
   </si>
   <si>
+    <t>www.her2treatment.com</t>
+  </si>
+  <si>
     <t>www.her2treatmentoptions.com</t>
   </si>
   <si>
@@ -611,6 +614,9 @@
     <t>URL91</t>
   </si>
   <si>
+    <t>OFF</t>
+  </si>
+  <si>
     <t>HER2+ Breast Cancer Treatment | PERJETA® (pertuzumab)</t>
   </si>
   <si>
@@ -621,9 +627,6 @@
   </si>
   <si>
     <t>https://www.actemrainfo.com/</t>
-  </si>
-  <si>
-    <t>https://www.her2treatment.com</t>
   </si>
 </sst>
 </file>
@@ -1330,8 +1333,8 @@
   <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C28"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G88" sqref="G88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1363,7 +1366,7 @@
         <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -1377,7 +1380,7 @@
         <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -1388,10 +1391,10 @@
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -1433,10 +1436,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C7" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1467,7 +1470,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>20</v>
@@ -1481,7 +1484,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>20</v>
@@ -1495,7 +1498,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>20</v>
@@ -1503,13 +1506,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>20</v>
@@ -1520,10 +1523,10 @@
         <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="D13" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>20</v>
@@ -1537,7 +1540,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>20</v>
@@ -1551,7 +1554,7 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>20</v>
@@ -1565,7 +1568,7 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>20</v>
@@ -1579,7 +1582,7 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>20</v>
@@ -1593,7 +1596,7 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>20</v>
@@ -1607,7 +1610,7 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>20</v>
@@ -1618,10 +1621,10 @@
         <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="D20" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>20</v>
@@ -1635,7 +1638,7 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>20</v>
@@ -1649,7 +1652,7 @@
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>20</v>
@@ -1663,7 +1666,7 @@
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>20</v>
@@ -1677,7 +1680,7 @@
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>20</v>
@@ -1691,7 +1694,7 @@
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>20</v>
@@ -1705,7 +1708,7 @@
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>20</v>
@@ -1719,7 +1722,7 @@
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>20</v>
@@ -1733,7 +1736,7 @@
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>20</v>
@@ -1747,7 +1750,7 @@
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>20</v>
@@ -1761,7 +1764,7 @@
         <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>20</v>
@@ -1775,7 +1778,7 @@
         <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>20</v>
@@ -1789,7 +1792,7 @@
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>20</v>
@@ -1803,7 +1806,7 @@
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>20</v>
@@ -1817,7 +1820,7 @@
         <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>20</v>
@@ -1831,7 +1834,7 @@
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>20</v>
@@ -1845,7 +1848,7 @@
         <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>20</v>
@@ -1856,10 +1859,10 @@
         <v>57</v>
       </c>
       <c r="C37" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="D37" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>20</v>
@@ -1873,7 +1876,7 @@
         <v>0</v>
       </c>
       <c r="D38" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>20</v>
@@ -1887,7 +1890,7 @@
         <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>20</v>
@@ -1901,7 +1904,7 @@
         <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>20</v>
@@ -1915,7 +1918,7 @@
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>20</v>
@@ -1929,7 +1932,7 @@
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>20</v>
@@ -1937,13 +1940,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>200</v>
+        <v>63</v>
       </c>
       <c r="C43" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="D43" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>20</v>
@@ -1951,13 +1954,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C44" t="s">
         <v>0</v>
       </c>
       <c r="D44" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>20</v>
@@ -1965,13 +1968,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C45" t="s">
         <v>0</v>
       </c>
       <c r="D45" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>20</v>
@@ -1979,13 +1982,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C46" t="s">
         <v>0</v>
       </c>
       <c r="D46" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>20</v>
@@ -1993,13 +1996,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C47" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="D47" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>20</v>
@@ -2007,13 +2010,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C48" t="s">
         <v>0</v>
       </c>
       <c r="D48" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>20</v>
@@ -2021,13 +2024,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C49" t="s">
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>20</v>
@@ -2035,13 +2038,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C50" t="s">
         <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>20</v>
@@ -2049,13 +2052,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C51" t="s">
         <v>0</v>
       </c>
       <c r="D51" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>20</v>
@@ -2063,13 +2066,13 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C52" t="s">
         <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>20</v>
@@ -2077,13 +2080,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C53" t="s">
         <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>20</v>
@@ -2091,13 +2094,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C54" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="D54" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>20</v>
@@ -2105,13 +2108,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C55" t="s">
         <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>20</v>
@@ -2119,13 +2122,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C56" t="s">
         <v>0</v>
       </c>
       <c r="D56" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>20</v>
@@ -2133,13 +2136,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C57" t="s">
         <v>0</v>
       </c>
       <c r="D57" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>20</v>
@@ -2147,13 +2150,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C58" t="s">
         <v>0</v>
       </c>
       <c r="D58" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>20</v>
@@ -2161,13 +2164,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C59" t="s">
         <v>0</v>
       </c>
       <c r="D59" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E59" s="6" t="s">
         <v>20</v>
@@ -2175,13 +2178,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C60" t="s">
         <v>0</v>
       </c>
       <c r="D60" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>20</v>
@@ -2189,13 +2192,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C61" t="s">
         <v>0</v>
       </c>
       <c r="D61" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>20</v>
@@ -2203,13 +2206,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C62" t="s">
         <v>0</v>
       </c>
       <c r="D62" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E62" s="6" t="s">
         <v>20</v>
@@ -2217,13 +2220,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C63" t="s">
         <v>0</v>
       </c>
       <c r="D63" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>20</v>
@@ -2231,13 +2234,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C64" t="s">
         <v>0</v>
       </c>
       <c r="D64" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>20</v>
@@ -2245,13 +2248,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C65" t="s">
         <v>0</v>
       </c>
       <c r="D65" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>20</v>
@@ -2259,13 +2262,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C66" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="D66" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>20</v>
@@ -2273,13 +2276,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C67" t="s">
         <v>0</v>
       </c>
       <c r="D67" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>20</v>
@@ -2287,13 +2290,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C68" t="s">
         <v>0</v>
       </c>
       <c r="D68" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>20</v>
@@ -2301,13 +2304,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C69" t="s">
         <v>0</v>
       </c>
       <c r="D69" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E69" s="6" t="s">
         <v>20</v>
@@ -2315,13 +2318,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C70" t="s">
         <v>0</v>
       </c>
       <c r="D70" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>20</v>
@@ -2329,13 +2332,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C71" t="s">
         <v>0</v>
       </c>
       <c r="D71" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E71" s="6" t="s">
         <v>20</v>
@@ -2343,13 +2346,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C72" t="s">
         <v>0</v>
       </c>
       <c r="D72" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E72" s="6" t="s">
         <v>20</v>
@@ -2357,13 +2360,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C73" t="s">
         <v>0</v>
       </c>
       <c r="D73" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E73" s="6" t="s">
         <v>20</v>
@@ -2371,13 +2374,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="13" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C74" t="s">
         <v>0</v>
       </c>
       <c r="D74" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E74" s="6" t="s">
         <v>20</v>
@@ -2385,13 +2388,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C75" t="s">
         <v>0</v>
       </c>
       <c r="D75" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E75" s="6" t="s">
         <v>20</v>
@@ -2399,13 +2402,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C76" t="s">
         <v>0</v>
       </c>
       <c r="D76" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>20</v>
@@ -2413,13 +2416,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C77" t="s">
         <v>0</v>
       </c>
       <c r="D77" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E77" s="6" t="s">
         <v>20</v>
@@ -2427,13 +2430,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C78" t="s">
         <v>0</v>
       </c>
       <c r="D78" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E78" s="6" t="s">
         <v>20</v>
@@ -2441,13 +2444,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C79" t="s">
         <v>0</v>
       </c>
       <c r="D79" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E79" s="6" t="s">
         <v>20</v>
@@ -2455,13 +2458,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C80" t="s">
         <v>0</v>
       </c>
       <c r="D80" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E80" s="6" t="s">
         <v>20</v>
@@ -2469,13 +2472,13 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C81" t="s">
         <v>0</v>
       </c>
       <c r="D81" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E81" s="6" t="s">
         <v>20</v>
@@ -2483,13 +2486,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C82" t="s">
         <v>0</v>
       </c>
       <c r="D82" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E82" s="6" t="s">
         <v>20</v>
@@ -2497,13 +2500,13 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C83" t="s">
         <v>0</v>
       </c>
       <c r="D83" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E83" s="6" t="s">
         <v>20</v>
@@ -2511,13 +2514,13 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C84" t="s">
         <v>0</v>
       </c>
       <c r="D84" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E84" s="6" t="s">
         <v>20</v>
@@ -2525,13 +2528,13 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C85" t="s">
         <v>0</v>
       </c>
       <c r="D85" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E85" s="6" t="s">
         <v>20</v>
@@ -2539,13 +2542,13 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C86" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="D86" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E86" s="6" t="s">
         <v>20</v>
@@ -2553,13 +2556,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C87" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="D87" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E87" s="6" t="s">
         <v>20</v>
@@ -2567,13 +2570,13 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C88" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="D88" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E88" s="6" t="s">
         <v>20</v>
@@ -2581,13 +2584,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C89" t="s">
         <v>0</v>
       </c>
       <c r="D89" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E89" s="6" t="s">
         <v>20</v>
@@ -2595,13 +2598,13 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C90" t="s">
         <v>0</v>
       </c>
       <c r="D90" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E90" s="6" t="s">
         <v>20</v>
@@ -2609,13 +2612,13 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C91" t="s">
         <v>0</v>
       </c>
       <c r="D91" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E91" s="6" t="s">
         <v>20</v>
@@ -2623,13 +2626,13 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C92" t="s">
         <v>0</v>
       </c>
       <c r="D92" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E92" s="6" t="s">
         <v>20</v>
@@ -2667,7 +2670,7 @@
     <hyperlink ref="A39" r:id="rId28" display="http://www.genentech-pro.com/"/>
     <hyperlink ref="A40" r:id="rId29" display="http://www.hemework.com/"/>
     <hyperlink ref="A41" r:id="rId30" display="http://www.hemlibra.com/"/>
-    <hyperlink ref="A43" r:id="rId31"/>
+    <hyperlink ref="A43" r:id="rId31" display="http://www.her2treatment.com/"/>
     <hyperlink ref="A44" r:id="rId32" display="http://www.her2treatmentoptions.com/"/>
     <hyperlink ref="A45" r:id="rId33" display="http://www.herceptin.com/"/>
     <hyperlink ref="A46" r:id="rId34" display="http://www.herceptinhylecta.com/"/>

</xml_diff>

<commit_message>
19 Nov 2021 Commit
</commit_message>
<xml_diff>
--- a/src/main/java/ccpa/testdata/TestDataCCPA.xlsx
+++ b/src/main/java/ccpa/testdata/TestDataCCPA.xlsx
@@ -212,9 +212,6 @@
     <t>www.hemlibra-hcp.com</t>
   </si>
   <si>
-    <t>www.her2treatment.com</t>
-  </si>
-  <si>
     <t>www.her2treatmentoptions.com</t>
   </si>
   <si>
@@ -614,19 +611,22 @@
     <t>URL91</t>
   </si>
   <si>
+    <t>HER2+ Breast Cancer Treatment | PERJETA® (pertuzumab)</t>
+  </si>
+  <si>
+    <t>https://www.perjeta.com/</t>
+  </si>
+  <si>
+    <t>https://www.biomarkertesting.com/</t>
+  </si>
+  <si>
+    <t>https://www.actemrainfo.com/</t>
+  </si>
+  <si>
+    <t>https://www.her2treatment.com</t>
+  </si>
+  <si>
     <t>OFF</t>
-  </si>
-  <si>
-    <t>HER2+ Breast Cancer Treatment | PERJETA® (pertuzumab)</t>
-  </si>
-  <si>
-    <t>https://www.perjeta.com/</t>
-  </si>
-  <si>
-    <t>https://www.biomarkertesting.com/</t>
-  </si>
-  <si>
-    <t>https://www.actemrainfo.com/</t>
   </si>
 </sst>
 </file>
@@ -994,7 +994,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1333,8 +1333,8 @@
   <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G88" sqref="G88"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1366,7 +1366,7 @@
         <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -1380,7 +1380,7 @@
         <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -1391,13 +1391,13 @@
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C4" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -1411,7 +1411,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -1425,7 +1425,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>8</v>
@@ -1436,10 +1436,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C7" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1453,7 +1453,7 @@
         <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1467,10 +1467,10 @@
         <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>20</v>
@@ -1481,10 +1481,10 @@
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>20</v>
@@ -1495,10 +1495,10 @@
         <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>20</v>
@@ -1506,13 +1506,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C12" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>20</v>
@@ -1523,10 +1523,10 @@
         <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>20</v>
@@ -1537,10 +1537,10 @@
         <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>20</v>
@@ -1551,10 +1551,10 @@
         <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>20</v>
@@ -1565,10 +1565,10 @@
         <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>20</v>
@@ -1579,10 +1579,10 @@
         <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>20</v>
@@ -1593,10 +1593,10 @@
         <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>20</v>
@@ -1607,10 +1607,10 @@
         <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>20</v>
@@ -1621,10 +1621,10 @@
         <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>20</v>
@@ -1635,10 +1635,10 @@
         <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>20</v>
@@ -1649,10 +1649,10 @@
         <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>20</v>
@@ -1663,10 +1663,10 @@
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>20</v>
@@ -1677,10 +1677,10 @@
         <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>20</v>
@@ -1691,10 +1691,10 @@
         <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>20</v>
@@ -1705,10 +1705,10 @@
         <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>20</v>
@@ -1719,10 +1719,10 @@
         <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>20</v>
@@ -1733,10 +1733,10 @@
         <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>20</v>
@@ -1747,10 +1747,10 @@
         <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>20</v>
@@ -1761,10 +1761,10 @@
         <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>20</v>
@@ -1775,10 +1775,10 @@
         <v>51</v>
       </c>
       <c r="C31" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>20</v>
@@ -1789,10 +1789,10 @@
         <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>20</v>
@@ -1803,10 +1803,10 @@
         <v>53</v>
       </c>
       <c r="C33" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>20</v>
@@ -1817,10 +1817,10 @@
         <v>54</v>
       </c>
       <c r="C34" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>20</v>
@@ -1831,10 +1831,10 @@
         <v>55</v>
       </c>
       <c r="C35" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D35" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>20</v>
@@ -1845,10 +1845,10 @@
         <v>56</v>
       </c>
       <c r="C36" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>20</v>
@@ -1859,10 +1859,10 @@
         <v>57</v>
       </c>
       <c r="C37" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>20</v>
@@ -1873,10 +1873,10 @@
         <v>58</v>
       </c>
       <c r="C38" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>20</v>
@@ -1887,10 +1887,10 @@
         <v>59</v>
       </c>
       <c r="C39" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>20</v>
@@ -1901,10 +1901,10 @@
         <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>20</v>
@@ -1915,10 +1915,10 @@
         <v>61</v>
       </c>
       <c r="C41" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>20</v>
@@ -1929,10 +1929,10 @@
         <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D42" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>20</v>
@@ -1940,13 +1940,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>63</v>
+        <v>200</v>
       </c>
       <c r="C43" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D43" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>20</v>
@@ -1954,13 +1954,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C44" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D44" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>20</v>
@@ -1968,13 +1968,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C45" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D45" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>20</v>
@@ -1982,13 +1982,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C46" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D46" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>20</v>
@@ -1996,13 +1996,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C47" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D47" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>20</v>
@@ -2010,13 +2010,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C48" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D48" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>20</v>
@@ -2024,13 +2024,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C49" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>20</v>
@@ -2038,13 +2038,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C50" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D50" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>20</v>
@@ -2052,13 +2052,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C51" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D51" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>20</v>
@@ -2066,13 +2066,13 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C52" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D52" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>20</v>
@@ -2080,13 +2080,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C53" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D53" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>20</v>
@@ -2094,13 +2094,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C54" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>20</v>
@@ -2108,13 +2108,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C55" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D55" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>20</v>
@@ -2122,13 +2122,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C56" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D56" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>20</v>
@@ -2136,13 +2136,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C57" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D57" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>20</v>
@@ -2150,13 +2150,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C58" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D58" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>20</v>
@@ -2164,13 +2164,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C59" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D59" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E59" s="6" t="s">
         <v>20</v>
@@ -2178,13 +2178,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C60" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D60" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>20</v>
@@ -2192,13 +2192,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C61" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D61" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>20</v>
@@ -2206,13 +2206,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C62" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D62" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E62" s="6" t="s">
         <v>20</v>
@@ -2220,13 +2220,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C63" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D63" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>20</v>
@@ -2234,13 +2234,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C64" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D64" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>20</v>
@@ -2248,13 +2248,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C65" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D65" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>20</v>
@@ -2262,13 +2262,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C66" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D66" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>20</v>
@@ -2276,13 +2276,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C67" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D67" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>20</v>
@@ -2290,13 +2290,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C68" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D68" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>20</v>
@@ -2304,13 +2304,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C69" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D69" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E69" s="6" t="s">
         <v>20</v>
@@ -2318,13 +2318,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C70" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D70" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>20</v>
@@ -2332,13 +2332,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C71" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D71" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E71" s="6" t="s">
         <v>20</v>
@@ -2346,13 +2346,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C72" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D72" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E72" s="6" t="s">
         <v>20</v>
@@ -2360,13 +2360,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C73" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D73" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E73" s="6" t="s">
         <v>20</v>
@@ -2374,13 +2374,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C74" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D74" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E74" s="6" t="s">
         <v>20</v>
@@ -2388,13 +2388,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C75" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D75" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E75" s="6" t="s">
         <v>20</v>
@@ -2402,13 +2402,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C76" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D76" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>20</v>
@@ -2416,13 +2416,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C77" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D77" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E77" s="6" t="s">
         <v>20</v>
@@ -2430,13 +2430,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C78" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D78" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E78" s="6" t="s">
         <v>20</v>
@@ -2444,13 +2444,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C79" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D79" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E79" s="6" t="s">
         <v>20</v>
@@ -2458,13 +2458,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C80" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D80" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E80" s="6" t="s">
         <v>20</v>
@@ -2472,13 +2472,13 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C81" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D81" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E81" s="6" t="s">
         <v>20</v>
@@ -2486,13 +2486,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C82" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D82" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E82" s="6" t="s">
         <v>20</v>
@@ -2500,13 +2500,13 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C83" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D83" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E83" s="6" t="s">
         <v>20</v>
@@ -2514,13 +2514,13 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C84" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D84" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E84" s="6" t="s">
         <v>20</v>
@@ -2528,13 +2528,13 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C85" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D85" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E85" s="6" t="s">
         <v>20</v>
@@ -2542,13 +2542,13 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C86" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D86" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E86" s="6" t="s">
         <v>20</v>
@@ -2556,13 +2556,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C87" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D87" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E87" s="6" t="s">
         <v>20</v>
@@ -2570,13 +2570,13 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C88" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="D88" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E88" s="6" t="s">
         <v>20</v>
@@ -2584,13 +2584,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C89" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D89" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E89" s="6" t="s">
         <v>20</v>
@@ -2598,13 +2598,13 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C90" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D90" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E90" s="6" t="s">
         <v>20</v>
@@ -2612,13 +2612,13 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C91" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D91" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E91" s="6" t="s">
         <v>20</v>
@@ -2626,13 +2626,13 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C92" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D92" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E92" s="6" t="s">
         <v>20</v>
@@ -2670,7 +2670,7 @@
     <hyperlink ref="A39" r:id="rId28" display="http://www.genentech-pro.com/"/>
     <hyperlink ref="A40" r:id="rId29" display="http://www.hemework.com/"/>
     <hyperlink ref="A41" r:id="rId30" display="http://www.hemlibra.com/"/>
-    <hyperlink ref="A43" r:id="rId31" display="http://www.her2treatment.com/"/>
+    <hyperlink ref="A43" r:id="rId31"/>
     <hyperlink ref="A44" r:id="rId32" display="http://www.her2treatmentoptions.com/"/>
     <hyperlink ref="A45" r:id="rId33" display="http://www.herceptin.com/"/>
     <hyperlink ref="A46" r:id="rId34" display="http://www.herceptinhylecta.com/"/>

</xml_diff>

<commit_message>
22 Nov 2021 commit
</commit_message>
<xml_diff>
--- a/src/main/java/ccpa/testdata/TestDataCCPA.xlsx
+++ b/src/main/java/ccpa/testdata/TestDataCCPA.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="201">
   <si>
     <t>ON</t>
   </si>
@@ -624,9 +624,6 @@
   </si>
   <si>
     <t>https://www.her2treatment.com</t>
-  </si>
-  <si>
-    <t>OFF</t>
   </si>
 </sst>
 </file>
@@ -994,7 +991,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1333,8 +1330,8 @@
   <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F87" sqref="F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1397,7 +1394,7 @@
         <v>196</v>
       </c>
       <c r="C4" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -1411,7 +1408,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -1425,7 +1422,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>8</v>
@@ -1453,7 +1450,7 @@
         <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1467,7 +1464,7 @@
         <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
         <v>112</v>
@@ -1481,7 +1478,7 @@
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
         <v>113</v>
@@ -1495,7 +1492,7 @@
         <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
         <v>114</v>
@@ -1509,7 +1506,7 @@
         <v>198</v>
       </c>
       <c r="C12" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
         <v>115</v>
@@ -1537,7 +1534,7 @@
         <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D14" t="s">
         <v>117</v>
@@ -1551,7 +1548,7 @@
         <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D15" t="s">
         <v>118</v>
@@ -1565,7 +1562,7 @@
         <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D16" t="s">
         <v>119</v>
@@ -1579,7 +1576,7 @@
         <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D17" t="s">
         <v>120</v>
@@ -1593,7 +1590,7 @@
         <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D18" t="s">
         <v>121</v>
@@ -1607,7 +1604,7 @@
         <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D19" t="s">
         <v>122</v>
@@ -1635,7 +1632,7 @@
         <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D21" t="s">
         <v>124</v>
@@ -1649,7 +1646,7 @@
         <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D22" t="s">
         <v>125</v>
@@ -1663,7 +1660,7 @@
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D23" t="s">
         <v>126</v>
@@ -1677,7 +1674,7 @@
         <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D24" t="s">
         <v>127</v>
@@ -1691,7 +1688,7 @@
         <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D25" t="s">
         <v>128</v>
@@ -1705,7 +1702,7 @@
         <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D26" t="s">
         <v>129</v>
@@ -1719,7 +1716,7 @@
         <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D27" t="s">
         <v>130</v>
@@ -1733,7 +1730,7 @@
         <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D28" t="s">
         <v>131</v>
@@ -1747,7 +1744,7 @@
         <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D29" t="s">
         <v>132</v>
@@ -1761,7 +1758,7 @@
         <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D30" t="s">
         <v>133</v>
@@ -1775,7 +1772,7 @@
         <v>51</v>
       </c>
       <c r="C31" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D31" t="s">
         <v>134</v>
@@ -1789,7 +1786,7 @@
         <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D32" t="s">
         <v>135</v>
@@ -1803,7 +1800,7 @@
         <v>53</v>
       </c>
       <c r="C33" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D33" t="s">
         <v>136</v>
@@ -1817,7 +1814,7 @@
         <v>54</v>
       </c>
       <c r="C34" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D34" t="s">
         <v>137</v>
@@ -1831,7 +1828,7 @@
         <v>55</v>
       </c>
       <c r="C35" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D35" t="s">
         <v>138</v>
@@ -1845,7 +1842,7 @@
         <v>56</v>
       </c>
       <c r="C36" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D36" t="s">
         <v>139</v>
@@ -1873,7 +1870,7 @@
         <v>58</v>
       </c>
       <c r="C38" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D38" t="s">
         <v>141</v>
@@ -1887,7 +1884,7 @@
         <v>59</v>
       </c>
       <c r="C39" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D39" t="s">
         <v>142</v>
@@ -1901,7 +1898,7 @@
         <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D40" t="s">
         <v>143</v>
@@ -1915,7 +1912,7 @@
         <v>61</v>
       </c>
       <c r="C41" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D41" t="s">
         <v>144</v>
@@ -1929,7 +1926,7 @@
         <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D42" t="s">
         <v>145</v>
@@ -1957,7 +1954,7 @@
         <v>63</v>
       </c>
       <c r="C44" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D44" t="s">
         <v>147</v>
@@ -1971,7 +1968,7 @@
         <v>64</v>
       </c>
       <c r="C45" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D45" t="s">
         <v>148</v>
@@ -1985,7 +1982,7 @@
         <v>65</v>
       </c>
       <c r="C46" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D46" t="s">
         <v>149</v>
@@ -2013,7 +2010,7 @@
         <v>67</v>
       </c>
       <c r="C48" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D48" t="s">
         <v>151</v>
@@ -2027,7 +2024,7 @@
         <v>68</v>
       </c>
       <c r="C49" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D49" t="s">
         <v>152</v>
@@ -2041,7 +2038,7 @@
         <v>69</v>
       </c>
       <c r="C50" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D50" t="s">
         <v>153</v>
@@ -2055,7 +2052,7 @@
         <v>70</v>
       </c>
       <c r="C51" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D51" t="s">
         <v>154</v>
@@ -2069,7 +2066,7 @@
         <v>71</v>
       </c>
       <c r="C52" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D52" t="s">
         <v>155</v>
@@ -2083,7 +2080,7 @@
         <v>72</v>
       </c>
       <c r="C53" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D53" t="s">
         <v>156</v>
@@ -2111,7 +2108,7 @@
         <v>74</v>
       </c>
       <c r="C55" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D55" t="s">
         <v>158</v>
@@ -2125,7 +2122,7 @@
         <v>75</v>
       </c>
       <c r="C56" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D56" t="s">
         <v>159</v>
@@ -2139,7 +2136,7 @@
         <v>76</v>
       </c>
       <c r="C57" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D57" t="s">
         <v>160</v>
@@ -2153,7 +2150,7 @@
         <v>77</v>
       </c>
       <c r="C58" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D58" t="s">
         <v>161</v>
@@ -2167,7 +2164,7 @@
         <v>78</v>
       </c>
       <c r="C59" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D59" t="s">
         <v>162</v>
@@ -2181,7 +2178,7 @@
         <v>79</v>
       </c>
       <c r="C60" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D60" t="s">
         <v>163</v>
@@ -2195,7 +2192,7 @@
         <v>80</v>
       </c>
       <c r="C61" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D61" t="s">
         <v>164</v>
@@ -2209,7 +2206,7 @@
         <v>81</v>
       </c>
       <c r="C62" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D62" t="s">
         <v>165</v>
@@ -2223,7 +2220,7 @@
         <v>82</v>
       </c>
       <c r="C63" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D63" t="s">
         <v>166</v>
@@ -2237,7 +2234,7 @@
         <v>83</v>
       </c>
       <c r="C64" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D64" t="s">
         <v>167</v>
@@ -2251,7 +2248,7 @@
         <v>84</v>
       </c>
       <c r="C65" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D65" t="s">
         <v>168</v>
@@ -2279,7 +2276,7 @@
         <v>86</v>
       </c>
       <c r="C67" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D67" t="s">
         <v>170</v>
@@ -2293,7 +2290,7 @@
         <v>87</v>
       </c>
       <c r="C68" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D68" t="s">
         <v>171</v>
@@ -2307,7 +2304,7 @@
         <v>88</v>
       </c>
       <c r="C69" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D69" t="s">
         <v>172</v>
@@ -2321,7 +2318,7 @@
         <v>89</v>
       </c>
       <c r="C70" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D70" t="s">
         <v>173</v>
@@ -2335,7 +2332,7 @@
         <v>90</v>
       </c>
       <c r="C71" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D71" t="s">
         <v>174</v>
@@ -2349,7 +2346,7 @@
         <v>91</v>
       </c>
       <c r="C72" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D72" t="s">
         <v>175</v>
@@ -2363,7 +2360,7 @@
         <v>92</v>
       </c>
       <c r="C73" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D73" t="s">
         <v>176</v>
@@ -2377,7 +2374,7 @@
         <v>93</v>
       </c>
       <c r="C74" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D74" t="s">
         <v>177</v>
@@ -2391,7 +2388,7 @@
         <v>94</v>
       </c>
       <c r="C75" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D75" t="s">
         <v>178</v>
@@ -2405,7 +2402,7 @@
         <v>95</v>
       </c>
       <c r="C76" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D76" t="s">
         <v>179</v>
@@ -2419,7 +2416,7 @@
         <v>96</v>
       </c>
       <c r="C77" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D77" t="s">
         <v>180</v>
@@ -2433,7 +2430,7 @@
         <v>97</v>
       </c>
       <c r="C78" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D78" t="s">
         <v>181</v>
@@ -2447,7 +2444,7 @@
         <v>98</v>
       </c>
       <c r="C79" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D79" t="s">
         <v>182</v>
@@ -2461,7 +2458,7 @@
         <v>99</v>
       </c>
       <c r="C80" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D80" t="s">
         <v>183</v>
@@ -2475,7 +2472,7 @@
         <v>100</v>
       </c>
       <c r="C81" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D81" t="s">
         <v>184</v>
@@ -2489,7 +2486,7 @@
         <v>101</v>
       </c>
       <c r="C82" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D82" t="s">
         <v>185</v>
@@ -2503,7 +2500,7 @@
         <v>102</v>
       </c>
       <c r="C83" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D83" t="s">
         <v>186</v>
@@ -2517,7 +2514,7 @@
         <v>103</v>
       </c>
       <c r="C84" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D84" t="s">
         <v>187</v>
@@ -2531,7 +2528,7 @@
         <v>104</v>
       </c>
       <c r="C85" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D85" t="s">
         <v>188</v>
@@ -2587,7 +2584,7 @@
         <v>108</v>
       </c>
       <c r="C89" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D89" t="s">
         <v>192</v>
@@ -2601,7 +2598,7 @@
         <v>109</v>
       </c>
       <c r="C90" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D90" t="s">
         <v>193</v>
@@ -2615,7 +2612,7 @@
         <v>110</v>
       </c>
       <c r="C91" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D91" t="s">
         <v>194</v>
@@ -2629,7 +2626,7 @@
         <v>111</v>
       </c>
       <c r="C92" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D92" t="s">
         <v>195</v>

</xml_diff>

<commit_message>
23 Nov 2021 3rd commit
</commit_message>
<xml_diff>
--- a/src/main/java/ccpa/testdata/TestDataCCPA.xlsx
+++ b/src/main/java/ccpa/testdata/TestDataCCPA.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="202">
   <si>
     <t>ON</t>
   </si>
@@ -624,6 +624,9 @@
   </si>
   <si>
     <t>https://www.her2treatment.com</t>
+  </si>
+  <si>
+    <t>OFF</t>
   </si>
 </sst>
 </file>
@@ -991,7 +994,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1330,8 +1333,8 @@
   <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F87" sqref="F87"/>
+      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10:C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,7 +1481,7 @@
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D10" t="s">
         <v>113</v>
@@ -1492,7 +1495,7 @@
         <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D11" t="s">
         <v>114</v>
@@ -1506,7 +1509,7 @@
         <v>198</v>
       </c>
       <c r="C12" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D12" t="s">
         <v>115</v>
@@ -1520,7 +1523,7 @@
         <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D13" t="s">
         <v>116</v>
@@ -1534,7 +1537,7 @@
         <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D14" t="s">
         <v>117</v>
@@ -1548,7 +1551,7 @@
         <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D15" t="s">
         <v>118</v>
@@ -1562,7 +1565,7 @@
         <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D16" t="s">
         <v>119</v>
@@ -1576,7 +1579,7 @@
         <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D17" t="s">
         <v>120</v>
@@ -1590,7 +1593,7 @@
         <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D18" t="s">
         <v>121</v>
@@ -1604,7 +1607,7 @@
         <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D19" t="s">
         <v>122</v>
@@ -1618,7 +1621,7 @@
         <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D20" t="s">
         <v>123</v>
@@ -1632,7 +1635,7 @@
         <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D21" t="s">
         <v>124</v>
@@ -1646,7 +1649,7 @@
         <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D22" t="s">
         <v>125</v>
@@ -1660,7 +1663,7 @@
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D23" t="s">
         <v>126</v>
@@ -1674,7 +1677,7 @@
         <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D24" t="s">
         <v>127</v>
@@ -1688,7 +1691,7 @@
         <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D25" t="s">
         <v>128</v>
@@ -1702,7 +1705,7 @@
         <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D26" t="s">
         <v>129</v>
@@ -1716,7 +1719,7 @@
         <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D27" t="s">
         <v>130</v>
@@ -1730,7 +1733,7 @@
         <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D28" t="s">
         <v>131</v>
@@ -1744,7 +1747,7 @@
         <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D29" t="s">
         <v>132</v>
@@ -1758,7 +1761,7 @@
         <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D30" t="s">
         <v>133</v>
@@ -1772,7 +1775,7 @@
         <v>51</v>
       </c>
       <c r="C31" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D31" t="s">
         <v>134</v>
@@ -1786,7 +1789,7 @@
         <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D32" t="s">
         <v>135</v>
@@ -1800,7 +1803,7 @@
         <v>53</v>
       </c>
       <c r="C33" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D33" t="s">
         <v>136</v>
@@ -1814,7 +1817,7 @@
         <v>54</v>
       </c>
       <c r="C34" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D34" t="s">
         <v>137</v>
@@ -1828,7 +1831,7 @@
         <v>55</v>
       </c>
       <c r="C35" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D35" t="s">
         <v>138</v>
@@ -1842,7 +1845,7 @@
         <v>56</v>
       </c>
       <c r="C36" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D36" t="s">
         <v>139</v>
@@ -1856,7 +1859,7 @@
         <v>57</v>
       </c>
       <c r="C37" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D37" t="s">
         <v>140</v>
@@ -1870,7 +1873,7 @@
         <v>58</v>
       </c>
       <c r="C38" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D38" t="s">
         <v>141</v>
@@ -1884,7 +1887,7 @@
         <v>59</v>
       </c>
       <c r="C39" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D39" t="s">
         <v>142</v>
@@ -1898,7 +1901,7 @@
         <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D40" t="s">
         <v>143</v>
@@ -1912,7 +1915,7 @@
         <v>61</v>
       </c>
       <c r="C41" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D41" t="s">
         <v>144</v>
@@ -1926,7 +1929,7 @@
         <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D42" t="s">
         <v>145</v>
@@ -1940,7 +1943,7 @@
         <v>200</v>
       </c>
       <c r="C43" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D43" t="s">
         <v>146</v>
@@ -1954,7 +1957,7 @@
         <v>63</v>
       </c>
       <c r="C44" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D44" t="s">
         <v>147</v>
@@ -1968,7 +1971,7 @@
         <v>64</v>
       </c>
       <c r="C45" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D45" t="s">
         <v>148</v>
@@ -1982,7 +1985,7 @@
         <v>65</v>
       </c>
       <c r="C46" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D46" t="s">
         <v>149</v>
@@ -1996,7 +1999,7 @@
         <v>66</v>
       </c>
       <c r="C47" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D47" t="s">
         <v>150</v>
@@ -2010,7 +2013,7 @@
         <v>67</v>
       </c>
       <c r="C48" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D48" t="s">
         <v>151</v>
@@ -2024,7 +2027,7 @@
         <v>68</v>
       </c>
       <c r="C49" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D49" t="s">
         <v>152</v>
@@ -2038,7 +2041,7 @@
         <v>69</v>
       </c>
       <c r="C50" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D50" t="s">
         <v>153</v>
@@ -2052,7 +2055,7 @@
         <v>70</v>
       </c>
       <c r="C51" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D51" t="s">
         <v>154</v>
@@ -2066,7 +2069,7 @@
         <v>71</v>
       </c>
       <c r="C52" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D52" t="s">
         <v>155</v>
@@ -2080,7 +2083,7 @@
         <v>72</v>
       </c>
       <c r="C53" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D53" t="s">
         <v>156</v>
@@ -2094,7 +2097,7 @@
         <v>73</v>
       </c>
       <c r="C54" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D54" t="s">
         <v>157</v>
@@ -2108,7 +2111,7 @@
         <v>74</v>
       </c>
       <c r="C55" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D55" t="s">
         <v>158</v>
@@ -2122,7 +2125,7 @@
         <v>75</v>
       </c>
       <c r="C56" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D56" t="s">
         <v>159</v>
@@ -2136,7 +2139,7 @@
         <v>76</v>
       </c>
       <c r="C57" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D57" t="s">
         <v>160</v>
@@ -2150,7 +2153,7 @@
         <v>77</v>
       </c>
       <c r="C58" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D58" t="s">
         <v>161</v>
@@ -2164,7 +2167,7 @@
         <v>78</v>
       </c>
       <c r="C59" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D59" t="s">
         <v>162</v>
@@ -2178,7 +2181,7 @@
         <v>79</v>
       </c>
       <c r="C60" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D60" t="s">
         <v>163</v>
@@ -2192,7 +2195,7 @@
         <v>80</v>
       </c>
       <c r="C61" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D61" t="s">
         <v>164</v>
@@ -2206,7 +2209,7 @@
         <v>81</v>
       </c>
       <c r="C62" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D62" t="s">
         <v>165</v>
@@ -2220,7 +2223,7 @@
         <v>82</v>
       </c>
       <c r="C63" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D63" t="s">
         <v>166</v>
@@ -2234,7 +2237,7 @@
         <v>83</v>
       </c>
       <c r="C64" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D64" t="s">
         <v>167</v>
@@ -2248,7 +2251,7 @@
         <v>84</v>
       </c>
       <c r="C65" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D65" t="s">
         <v>168</v>
@@ -2262,7 +2265,7 @@
         <v>85</v>
       </c>
       <c r="C66" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D66" t="s">
         <v>169</v>
@@ -2276,7 +2279,7 @@
         <v>86</v>
       </c>
       <c r="C67" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D67" t="s">
         <v>170</v>
@@ -2290,7 +2293,7 @@
         <v>87</v>
       </c>
       <c r="C68" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D68" t="s">
         <v>171</v>
@@ -2304,7 +2307,7 @@
         <v>88</v>
       </c>
       <c r="C69" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D69" t="s">
         <v>172</v>
@@ -2318,7 +2321,7 @@
         <v>89</v>
       </c>
       <c r="C70" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D70" t="s">
         <v>173</v>
@@ -2332,7 +2335,7 @@
         <v>90</v>
       </c>
       <c r="C71" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D71" t="s">
         <v>174</v>
@@ -2346,7 +2349,7 @@
         <v>91</v>
       </c>
       <c r="C72" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D72" t="s">
         <v>175</v>
@@ -2360,7 +2363,7 @@
         <v>92</v>
       </c>
       <c r="C73" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D73" t="s">
         <v>176</v>
@@ -2374,7 +2377,7 @@
         <v>93</v>
       </c>
       <c r="C74" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D74" t="s">
         <v>177</v>
@@ -2388,7 +2391,7 @@
         <v>94</v>
       </c>
       <c r="C75" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D75" t="s">
         <v>178</v>
@@ -2402,7 +2405,7 @@
         <v>95</v>
       </c>
       <c r="C76" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D76" t="s">
         <v>179</v>
@@ -2416,7 +2419,7 @@
         <v>96</v>
       </c>
       <c r="C77" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D77" t="s">
         <v>180</v>
@@ -2430,7 +2433,7 @@
         <v>97</v>
       </c>
       <c r="C78" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D78" t="s">
         <v>181</v>
@@ -2444,7 +2447,7 @@
         <v>98</v>
       </c>
       <c r="C79" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D79" t="s">
         <v>182</v>
@@ -2458,7 +2461,7 @@
         <v>99</v>
       </c>
       <c r="C80" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D80" t="s">
         <v>183</v>
@@ -2472,7 +2475,7 @@
         <v>100</v>
       </c>
       <c r="C81" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D81" t="s">
         <v>184</v>
@@ -2486,7 +2489,7 @@
         <v>101</v>
       </c>
       <c r="C82" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D82" t="s">
         <v>185</v>
@@ -2500,7 +2503,7 @@
         <v>102</v>
       </c>
       <c r="C83" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D83" t="s">
         <v>186</v>
@@ -2514,7 +2517,7 @@
         <v>103</v>
       </c>
       <c r="C84" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D84" t="s">
         <v>187</v>
@@ -2528,7 +2531,7 @@
         <v>104</v>
       </c>
       <c r="C85" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D85" t="s">
         <v>188</v>
@@ -2542,7 +2545,7 @@
         <v>105</v>
       </c>
       <c r="C86" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D86" t="s">
         <v>189</v>
@@ -2556,7 +2559,7 @@
         <v>106</v>
       </c>
       <c r="C87" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D87" t="s">
         <v>190</v>
@@ -2570,7 +2573,7 @@
         <v>107</v>
       </c>
       <c r="C88" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D88" t="s">
         <v>191</v>
@@ -2584,7 +2587,7 @@
         <v>108</v>
       </c>
       <c r="C89" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D89" t="s">
         <v>192</v>
@@ -2598,7 +2601,7 @@
         <v>109</v>
       </c>
       <c r="C90" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D90" t="s">
         <v>193</v>
@@ -2612,7 +2615,7 @@
         <v>110</v>
       </c>
       <c r="C91" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D91" t="s">
         <v>194</v>
@@ -2626,7 +2629,7 @@
         <v>111</v>
       </c>
       <c r="C92" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="D92" t="s">
         <v>195</v>

</xml_diff>

<commit_message>
23 Nov 2021 4th commit
</commit_message>
<xml_diff>
--- a/src/main/java/ccpa/testdata/TestDataCCPA.xlsx
+++ b/src/main/java/ccpa/testdata/TestDataCCPA.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="201">
   <si>
     <t>ON</t>
   </si>
@@ -624,9 +624,6 @@
   </si>
   <si>
     <t>https://www.her2treatment.com</t>
-  </si>
-  <si>
-    <t>OFF</t>
   </si>
 </sst>
 </file>
@@ -994,7 +991,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1333,8 +1330,8 @@
   <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10:C92"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H83" sqref="H83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1481,7 +1478,7 @@
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
         <v>113</v>
@@ -1495,7 +1492,7 @@
         <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
         <v>114</v>
@@ -1509,7 +1506,7 @@
         <v>198</v>
       </c>
       <c r="C12" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
         <v>115</v>
@@ -1523,7 +1520,7 @@
         <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
         <v>116</v>
@@ -1537,7 +1534,7 @@
         <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D14" t="s">
         <v>117</v>
@@ -1551,7 +1548,7 @@
         <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D15" t="s">
         <v>118</v>
@@ -1565,7 +1562,7 @@
         <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D16" t="s">
         <v>119</v>
@@ -1579,7 +1576,7 @@
         <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D17" t="s">
         <v>120</v>
@@ -1593,7 +1590,7 @@
         <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D18" t="s">
         <v>121</v>
@@ -1607,7 +1604,7 @@
         <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D19" t="s">
         <v>122</v>
@@ -1621,7 +1618,7 @@
         <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
         <v>123</v>
@@ -1635,7 +1632,7 @@
         <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D21" t="s">
         <v>124</v>
@@ -1649,7 +1646,7 @@
         <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D22" t="s">
         <v>125</v>
@@ -1663,7 +1660,7 @@
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D23" t="s">
         <v>126</v>
@@ -1677,7 +1674,7 @@
         <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D24" t="s">
         <v>127</v>
@@ -1691,7 +1688,7 @@
         <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D25" t="s">
         <v>128</v>
@@ -1705,7 +1702,7 @@
         <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D26" t="s">
         <v>129</v>
@@ -1719,7 +1716,7 @@
         <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D27" t="s">
         <v>130</v>
@@ -1733,7 +1730,7 @@
         <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D28" t="s">
         <v>131</v>
@@ -1747,7 +1744,7 @@
         <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D29" t="s">
         <v>132</v>
@@ -1761,7 +1758,7 @@
         <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D30" t="s">
         <v>133</v>
@@ -1775,7 +1772,7 @@
         <v>51</v>
       </c>
       <c r="C31" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D31" t="s">
         <v>134</v>
@@ -1789,7 +1786,7 @@
         <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D32" t="s">
         <v>135</v>
@@ -1803,7 +1800,7 @@
         <v>53</v>
       </c>
       <c r="C33" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D33" t="s">
         <v>136</v>
@@ -1817,7 +1814,7 @@
         <v>54</v>
       </c>
       <c r="C34" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D34" t="s">
         <v>137</v>
@@ -1831,7 +1828,7 @@
         <v>55</v>
       </c>
       <c r="C35" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D35" t="s">
         <v>138</v>
@@ -1845,7 +1842,7 @@
         <v>56</v>
       </c>
       <c r="C36" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D36" t="s">
         <v>139</v>
@@ -1859,7 +1856,7 @@
         <v>57</v>
       </c>
       <c r="C37" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D37" t="s">
         <v>140</v>
@@ -1873,7 +1870,7 @@
         <v>58</v>
       </c>
       <c r="C38" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D38" t="s">
         <v>141</v>
@@ -1887,7 +1884,7 @@
         <v>59</v>
       </c>
       <c r="C39" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D39" t="s">
         <v>142</v>
@@ -1901,7 +1898,7 @@
         <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D40" t="s">
         <v>143</v>
@@ -1915,7 +1912,7 @@
         <v>61</v>
       </c>
       <c r="C41" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D41" t="s">
         <v>144</v>
@@ -1929,7 +1926,7 @@
         <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D42" t="s">
         <v>145</v>
@@ -1943,7 +1940,7 @@
         <v>200</v>
       </c>
       <c r="C43" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D43" t="s">
         <v>146</v>
@@ -1957,7 +1954,7 @@
         <v>63</v>
       </c>
       <c r="C44" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D44" t="s">
         <v>147</v>
@@ -1971,7 +1968,7 @@
         <v>64</v>
       </c>
       <c r="C45" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D45" t="s">
         <v>148</v>
@@ -1985,7 +1982,7 @@
         <v>65</v>
       </c>
       <c r="C46" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D46" t="s">
         <v>149</v>
@@ -1999,7 +1996,7 @@
         <v>66</v>
       </c>
       <c r="C47" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D47" t="s">
         <v>150</v>
@@ -2013,7 +2010,7 @@
         <v>67</v>
       </c>
       <c r="C48" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D48" t="s">
         <v>151</v>
@@ -2027,7 +2024,7 @@
         <v>68</v>
       </c>
       <c r="C49" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D49" t="s">
         <v>152</v>
@@ -2041,7 +2038,7 @@
         <v>69</v>
       </c>
       <c r="C50" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D50" t="s">
         <v>153</v>
@@ -2055,7 +2052,7 @@
         <v>70</v>
       </c>
       <c r="C51" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D51" t="s">
         <v>154</v>
@@ -2069,7 +2066,7 @@
         <v>71</v>
       </c>
       <c r="C52" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D52" t="s">
         <v>155</v>
@@ -2083,7 +2080,7 @@
         <v>72</v>
       </c>
       <c r="C53" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D53" t="s">
         <v>156</v>
@@ -2097,7 +2094,7 @@
         <v>73</v>
       </c>
       <c r="C54" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D54" t="s">
         <v>157</v>
@@ -2111,7 +2108,7 @@
         <v>74</v>
       </c>
       <c r="C55" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D55" t="s">
         <v>158</v>
@@ -2125,7 +2122,7 @@
         <v>75</v>
       </c>
       <c r="C56" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D56" t="s">
         <v>159</v>
@@ -2139,7 +2136,7 @@
         <v>76</v>
       </c>
       <c r="C57" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D57" t="s">
         <v>160</v>
@@ -2153,7 +2150,7 @@
         <v>77</v>
       </c>
       <c r="C58" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D58" t="s">
         <v>161</v>
@@ -2167,7 +2164,7 @@
         <v>78</v>
       </c>
       <c r="C59" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D59" t="s">
         <v>162</v>
@@ -2181,7 +2178,7 @@
         <v>79</v>
       </c>
       <c r="C60" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D60" t="s">
         <v>163</v>
@@ -2195,7 +2192,7 @@
         <v>80</v>
       </c>
       <c r="C61" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D61" t="s">
         <v>164</v>
@@ -2209,7 +2206,7 @@
         <v>81</v>
       </c>
       <c r="C62" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D62" t="s">
         <v>165</v>
@@ -2223,7 +2220,7 @@
         <v>82</v>
       </c>
       <c r="C63" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D63" t="s">
         <v>166</v>
@@ -2237,7 +2234,7 @@
         <v>83</v>
       </c>
       <c r="C64" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D64" t="s">
         <v>167</v>
@@ -2251,7 +2248,7 @@
         <v>84</v>
       </c>
       <c r="C65" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D65" t="s">
         <v>168</v>
@@ -2265,7 +2262,7 @@
         <v>85</v>
       </c>
       <c r="C66" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D66" t="s">
         <v>169</v>
@@ -2279,7 +2276,7 @@
         <v>86</v>
       </c>
       <c r="C67" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D67" t="s">
         <v>170</v>
@@ -2293,7 +2290,7 @@
         <v>87</v>
       </c>
       <c r="C68" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D68" t="s">
         <v>171</v>
@@ -2307,7 +2304,7 @@
         <v>88</v>
       </c>
       <c r="C69" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D69" t="s">
         <v>172</v>
@@ -2321,7 +2318,7 @@
         <v>89</v>
       </c>
       <c r="C70" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D70" t="s">
         <v>173</v>
@@ -2335,7 +2332,7 @@
         <v>90</v>
       </c>
       <c r="C71" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D71" t="s">
         <v>174</v>
@@ -2349,7 +2346,7 @@
         <v>91</v>
       </c>
       <c r="C72" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D72" t="s">
         <v>175</v>
@@ -2363,7 +2360,7 @@
         <v>92</v>
       </c>
       <c r="C73" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D73" t="s">
         <v>176</v>
@@ -2377,7 +2374,7 @@
         <v>93</v>
       </c>
       <c r="C74" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D74" t="s">
         <v>177</v>
@@ -2391,7 +2388,7 @@
         <v>94</v>
       </c>
       <c r="C75" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D75" t="s">
         <v>178</v>
@@ -2405,7 +2402,7 @@
         <v>95</v>
       </c>
       <c r="C76" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D76" t="s">
         <v>179</v>
@@ -2419,7 +2416,7 @@
         <v>96</v>
       </c>
       <c r="C77" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D77" t="s">
         <v>180</v>
@@ -2433,7 +2430,7 @@
         <v>97</v>
       </c>
       <c r="C78" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D78" t="s">
         <v>181</v>
@@ -2447,7 +2444,7 @@
         <v>98</v>
       </c>
       <c r="C79" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D79" t="s">
         <v>182</v>
@@ -2461,7 +2458,7 @@
         <v>99</v>
       </c>
       <c r="C80" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D80" t="s">
         <v>183</v>
@@ -2475,7 +2472,7 @@
         <v>100</v>
       </c>
       <c r="C81" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D81" t="s">
         <v>184</v>
@@ -2489,7 +2486,7 @@
         <v>101</v>
       </c>
       <c r="C82" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D82" t="s">
         <v>185</v>
@@ -2503,7 +2500,7 @@
         <v>102</v>
       </c>
       <c r="C83" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D83" t="s">
         <v>186</v>
@@ -2517,7 +2514,7 @@
         <v>103</v>
       </c>
       <c r="C84" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D84" t="s">
         <v>187</v>
@@ -2531,7 +2528,7 @@
         <v>104</v>
       </c>
       <c r="C85" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D85" t="s">
         <v>188</v>
@@ -2545,7 +2542,7 @@
         <v>105</v>
       </c>
       <c r="C86" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D86" t="s">
         <v>189</v>
@@ -2559,7 +2556,7 @@
         <v>106</v>
       </c>
       <c r="C87" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D87" t="s">
         <v>190</v>
@@ -2573,7 +2570,7 @@
         <v>107</v>
       </c>
       <c r="C88" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D88" t="s">
         <v>191</v>
@@ -2587,7 +2584,7 @@
         <v>108</v>
       </c>
       <c r="C89" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D89" t="s">
         <v>192</v>
@@ -2601,7 +2598,7 @@
         <v>109</v>
       </c>
       <c r="C90" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D90" t="s">
         <v>193</v>
@@ -2615,7 +2612,7 @@
         <v>110</v>
       </c>
       <c r="C91" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D91" t="s">
         <v>194</v>
@@ -2629,7 +2626,7 @@
         <v>111</v>
       </c>
       <c r="C92" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D92" t="s">
         <v>195</v>

</xml_diff>